<commit_message>
added final permutation, convert key to ull
</commit_message>
<xml_diff>
--- a/Extras/Book2.xlsx
+++ b/Extras/Book2.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="FinalPermutation" sheetId="3" r:id="rId1"/>
+    <sheet name="InitialPermutation" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="65">
   <si>
     <t>1</t>
   </si>
@@ -541,8 +542,801 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="66.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="42.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="str">
+        <f>"if (x &amp; (i &lt;&lt; "&amp;64-C1&amp;")) y |= (i &lt;&lt; "&amp;64-B1&amp;"); //Bit "&amp;C1&amp;" -&gt; "&amp;B1</f>
+        <v>if (x &amp; (i &lt;&lt; 24)) y |= (i &lt;&lt; 63); //Bit 40 -&gt; 1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="str">
+        <f t="shared" ref="A2:A64" si="0">"if (x &amp; (i &lt;&lt; "&amp;64-C2&amp;")) y |= (i &lt;&lt; "&amp;64-B2&amp;"); //Bit "&amp;C2&amp;" -&gt; "&amp;B2</f>
+        <v>if (x &amp; (i &lt;&lt; 56)) y |= (i &lt;&lt; 62); //Bit 8 -&gt; 2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 16)) y |= (i &lt;&lt; 61); //Bit 48 -&gt; 3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 48)) y |= (i &lt;&lt; 60); //Bit 16 -&gt; 4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 8)) y |= (i &lt;&lt; 59); //Bit 56 -&gt; 5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 40)) y |= (i &lt;&lt; 58); //Bit 24 -&gt; 6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 0)) y |= (i &lt;&lt; 57); //Bit 64 -&gt; 7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 32)) y |= (i &lt;&lt; 56); //Bit 32 -&gt; 8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 25)) y |= (i &lt;&lt; 55); //Bit 39 -&gt; 9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 57)) y |= (i &lt;&lt; 54); //Bit 7 -&gt; 10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 17)) y |= (i &lt;&lt; 53); //Bit 47 -&gt; 11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 49)) y |= (i &lt;&lt; 52); //Bit 15 -&gt; 12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 9)) y |= (i &lt;&lt; 51); //Bit 55 -&gt; 13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 41)) y |= (i &lt;&lt; 50); //Bit 23 -&gt; 14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 1)) y |= (i &lt;&lt; 49); //Bit 63 -&gt; 15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 33)) y |= (i &lt;&lt; 48); //Bit 31 -&gt; 16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 26)) y |= (i &lt;&lt; 47); //Bit 38 -&gt; 17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 58)) y |= (i &lt;&lt; 46); //Bit 6 -&gt; 18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 18)) y |= (i &lt;&lt; 45); //Bit 46 -&gt; 19</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 50)) y |= (i &lt;&lt; 44); //Bit 14 -&gt; 20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 10)) y |= (i &lt;&lt; 43); //Bit 54 -&gt; 21</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 42)) y |= (i &lt;&lt; 42); //Bit 22 -&gt; 22</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 2)) y |= (i &lt;&lt; 41); //Bit 62 -&gt; 23</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 34)) y |= (i &lt;&lt; 40); //Bit 30 -&gt; 24</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 27)) y |= (i &lt;&lt; 39); //Bit 37 -&gt; 25</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 59)) y |= (i &lt;&lt; 38); //Bit 5 -&gt; 26</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 19)) y |= (i &lt;&lt; 37); //Bit 45 -&gt; 27</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 51)) y |= (i &lt;&lt; 36); //Bit 13 -&gt; 28</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 11)) y |= (i &lt;&lt; 35); //Bit 53 -&gt; 29</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 43)) y |= (i &lt;&lt; 34); //Bit 21 -&gt; 30</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 3)) y |= (i &lt;&lt; 33); //Bit 61 -&gt; 31</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 35)) y |= (i &lt;&lt; 32); //Bit 29 -&gt; 32</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 28)) y |= (i &lt;&lt; 31); //Bit 36 -&gt; 33</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 60)) y |= (i &lt;&lt; 30); //Bit 4 -&gt; 34</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 20)) y |= (i &lt;&lt; 29); //Bit 44 -&gt; 35</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 52)) y |= (i &lt;&lt; 28); //Bit 12 -&gt; 36</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 12)) y |= (i &lt;&lt; 27); //Bit 52 -&gt; 37</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 44)) y |= (i &lt;&lt; 26); //Bit 20 -&gt; 38</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 4)) y |= (i &lt;&lt; 25); //Bit 60 -&gt; 39</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 36)) y |= (i &lt;&lt; 24); //Bit 28 -&gt; 40</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 30)) y |= (i &lt;&lt; 23); //Bit 34 -&gt; 41</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 61)) y |= (i &lt;&lt; 22); //Bit 3 -&gt; 42</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 21)) y |= (i &lt;&lt; 21); //Bit 43 -&gt; 43</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 53)) y |= (i &lt;&lt; 20); //Bit 11 -&gt; 44</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 13)) y |= (i &lt;&lt; 19); //Bit 51 -&gt; 45</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 45)) y |= (i &lt;&lt; 18); //Bit 19 -&gt; 46</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 5)) y |= (i &lt;&lt; 17); //Bit 59 -&gt; 47</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 37)) y |= (i &lt;&lt; 16); //Bit 27 -&gt; 48</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 30)) y |= (i &lt;&lt; 15); //Bit 34 -&gt; 49</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 62)) y |= (i &lt;&lt; 14); //Bit 2 -&gt; 50</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 22)) y |= (i &lt;&lt; 13); //Bit 42 -&gt; 51</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 54)) y |= (i &lt;&lt; 12); //Bit 10 -&gt; 52</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 14)) y |= (i &lt;&lt; 11); //Bit 50 -&gt; 53</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 46)) y |= (i &lt;&lt; 10); //Bit 18 -&gt; 54</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 6)) y |= (i &lt;&lt; 9); //Bit 58 -&gt; 55</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 38)) y |= (i &lt;&lt; 8); //Bit 26 -&gt; 56</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 31)) y |= (i &lt;&lt; 7); //Bit 33 -&gt; 57</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 63)) y |= (i &lt;&lt; 6); //Bit 1 -&gt; 58</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 23)) y |= (i &lt;&lt; 5); //Bit 41 -&gt; 59</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 55)) y |= (i &lt;&lt; 4); //Bit 9 -&gt; 60</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 15)) y |= (i &lt;&lt; 3); //Bit 49 -&gt; 61</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 47)) y |= (i &lt;&lt; 2); //Bit 17 -&gt; 62</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 7)) y |= (i &lt;&lt; 1); //Bit 57 -&gt; 63</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>if (x &amp; (i &lt;&lt; 39)) y |= (i &lt;&lt; 0); //Bit 25 -&gt; 64</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E64"/>
+  <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,12 +2124,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AN11" sqref="AN11"/>
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
working, fixed padding issue
</commit_message>
<xml_diff>
--- a/Extras/Book2.xlsx
+++ b/Extras/Book2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" firstSheet="3" activeTab="13"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="InitialPermutation" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,14 @@
     <sheet name="S6" sheetId="14" r:id="rId10"/>
     <sheet name="S7" sheetId="15" r:id="rId11"/>
     <sheet name="S8" sheetId="16" r:id="rId12"/>
-    <sheet name="PostS P-box" sheetId="17" r:id="rId13"/>
-    <sheet name="Sheet15" sheetId="18" r:id="rId14"/>
+    <sheet name="Sheet15" sheetId="18" r:id="rId13"/>
+    <sheet name="PostS P-box" sheetId="17" r:id="rId14"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId15"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId16"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId17"/>
     <sheet name="Sheet3" sheetId="7" r:id="rId18"/>
+    <sheet name="Sheet16" sheetId="19" r:id="rId19"/>
+    <sheet name="Sheet17" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="69">
   <si>
     <t>1</t>
   </si>
@@ -239,6 +241,15 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>001110</t>
+  </si>
+  <si>
+    <t>101011</t>
+  </si>
+  <si>
+    <t>001100</t>
   </si>
 </sst>
 </file>
@@ -571,7 +582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1066,14 +1079,14 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>if (x &amp; (i &lt;&lt; 23)) y |= (i &lt;&lt; 30); //Bit 41 -&gt; 34</v>
+        <f>"if (x &amp; (i &lt;&lt; "&amp;64-B41&amp;")) y |= (i &lt;&lt; "&amp;64-C41&amp;"); //Bit "&amp;B41&amp;" -&gt; "&amp;C41</f>
+        <v>if (x &amp; (i &lt;&lt; 23)) y |= (i &lt;&lt; 29); //Bit 41 -&gt; 35</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -4300,6 +4313,319 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="3.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1</v>
+      </c>
+      <c r="V2" s="1">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1</v>
+      </c>
+      <c r="X2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4796,319 +5122,6 @@
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="3.42578125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1">
-        <v>1</v>
-      </c>
-      <c r="L2" s="1">
-        <v>1</v>
-      </c>
-      <c r="M2" s="1">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1">
-        <v>1</v>
-      </c>
-      <c r="P2" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>1</v>
-      </c>
-      <c r="R2" s="1">
-        <v>0</v>
-      </c>
-      <c r="S2" s="1">
-        <v>1</v>
-      </c>
-      <c r="T2" s="1">
-        <v>0</v>
-      </c>
-      <c r="U2" s="1">
-        <v>1</v>
-      </c>
-      <c r="V2" s="1">
-        <v>0</v>
-      </c>
-      <c r="W2" s="1">
-        <v>1</v>
-      </c>
-      <c r="X2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
-      <c r="P3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>1</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0</v>
-      </c>
-      <c r="S3" s="1">
-        <v>0</v>
-      </c>
-      <c r="T3" s="1">
-        <v>0</v>
-      </c>
-      <c r="U3" s="1">
-        <v>0</v>
-      </c>
-      <c r="V3" s="1">
-        <v>1</v>
-      </c>
-      <c r="W3" s="1">
-        <v>0</v>
-      </c>
-      <c r="X3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="1">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7446,12 +7459,468 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AV3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AU3" sqref="AU3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="4.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1</v>
+      </c>
+      <c r="X2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1</v>
+      </c>
+      <c r="W3" s="1">
+        <v>1</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7948,13 +8417,13 @@
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>if (x &amp; (i &lt;&lt; 30)) y |= (i &lt;&lt; 23); //Bit 34 -&gt; 41</v>
+        <v>if (x &amp; (i &lt;&lt; 29)) y |= (i &lt;&lt; 23); //Bit 35 -&gt; 41</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -8236,6 +8705,77 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>111000</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="1">
+        <v>110100</v>
+      </c>
+      <c r="F1" s="1">
+        <v>111100</v>
+      </c>
+      <c r="G1" s="1">
+        <v>100000</v>
+      </c>
+      <c r="H1" s="1">
+        <v>110111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -9905,8 +10445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>